<commit_message>
update plaster_materials, added test and bug fixes
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/Plaster.xlsx
+++ b/delphin_6_automation/sampling/input_files/Plaster.xlsx
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Material ID</t>
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Lime Cement Mortar (High Cement Ratio)</t>
+  </si>
+  <si>
+    <t>Lime Cement Mortar (Low Cement Ratio)</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,10 +392,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2">
+        <v>717</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2">
+        <v>718</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>

</xml_diff>